<commit_message>
Re-add restriction help row
</commit_message>
<xml_diff>
--- a/spreadsheets/ghga_submission_minimal.xlsx
+++ b/spreadsheets/ghga_submission_minimal.xlsx
@@ -536,7 +536,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1005"/>
+  <dimension ref="A1:F1006"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -683,42 +683,66 @@
     <row r="5">
       <c r="A5" s="2" t="inlineStr">
         <is>
-          <t>required</t>
+          <t>unrestricted</t>
         </is>
       </c>
       <c r="B5" s="2" t="inlineStr">
         <is>
-          <t>required</t>
+          <t>unrestricted</t>
         </is>
       </c>
       <c r="C5" s="2" t="inlineStr">
         <is>
-          <t>required</t>
+          <t>unrestricted</t>
         </is>
       </c>
       <c r="D5" s="2" t="inlineStr">
         <is>
-          <t>required</t>
+          <t>unrestricted</t>
         </is>
       </c>
       <c r="E5" s="2" t="inlineStr">
         <is>
-          <t>required</t>
+          <t>unrestricted</t>
         </is>
       </c>
       <c r="F5" s="2" t="inlineStr">
         <is>
+          <t>unrestricted</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="inlineStr">
+        <is>
+          <t>required</t>
+        </is>
+      </c>
+      <c r="B6" s="2" t="inlineStr">
+        <is>
+          <t>required</t>
+        </is>
+      </c>
+      <c r="C6" s="2" t="inlineStr">
+        <is>
+          <t>required</t>
+        </is>
+      </c>
+      <c r="D6" s="2" t="inlineStr">
+        <is>
+          <t>required</t>
+        </is>
+      </c>
+      <c r="E6" s="2" t="inlineStr">
+        <is>
+          <t>required</t>
+        </is>
+      </c>
+      <c r="F6" s="2" t="inlineStr">
+        <is>
           <t>optional</t>
         </is>
       </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="3" t="n"/>
-      <c r="B6" s="3" t="n"/>
-      <c r="C6" s="3" t="n"/>
-      <c r="D6" s="3" t="n"/>
-      <c r="E6" s="3" t="n"/>
-      <c r="F6" s="3" t="n"/>
     </row>
     <row r="7">
       <c r="A7" s="3" t="n"/>
@@ -8711,6 +8735,14 @@
       <c r="D1005" s="3" t="n"/>
       <c r="E1005" s="3" t="n"/>
       <c r="F1005" s="3" t="n"/>
+    </row>
+    <row r="1006">
+      <c r="A1006" s="3" t="n"/>
+      <c r="B1006" s="3" t="n"/>
+      <c r="C1006" s="3" t="n"/>
+      <c r="D1006" s="3" t="n"/>
+      <c r="E1006" s="3" t="n"/>
+      <c r="F1006" s="3" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -8724,7 +8756,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I1005"/>
+  <dimension ref="A1:I1006"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8934,60 +8966,96 @@
     <row r="5">
       <c r="A5" s="5" t="inlineStr">
         <is>
-          <t>required</t>
+          <t>unrestricted</t>
         </is>
       </c>
       <c r="B5" s="5" t="inlineStr">
         <is>
-          <t>required</t>
+          <t>unrestricted</t>
         </is>
       </c>
       <c r="C5" s="5" t="inlineStr">
         <is>
-          <t>required</t>
+          <t>unrestricted</t>
         </is>
       </c>
       <c r="D5" s="5" t="inlineStr">
         <is>
-          <t>required</t>
+          <t>unrestricted</t>
         </is>
       </c>
       <c r="E5" s="5" t="inlineStr">
         <is>
-          <t>required</t>
+          <t>unrestricted</t>
         </is>
       </c>
       <c r="F5" s="5" t="inlineStr">
         <is>
-          <t>required</t>
+          <t>unrestricted</t>
         </is>
       </c>
       <c r="G5" s="5" t="inlineStr">
         <is>
-          <t>required</t>
+          <t>unrestricted</t>
         </is>
       </c>
       <c r="H5" s="5" t="inlineStr">
         <is>
-          <t>required</t>
+          <t>unrestricted</t>
         </is>
       </c>
       <c r="I5" s="5" t="inlineStr">
         <is>
+          <t>unrestricted</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="5" t="inlineStr">
+        <is>
+          <t>required</t>
+        </is>
+      </c>
+      <c r="B6" s="5" t="inlineStr">
+        <is>
+          <t>required</t>
+        </is>
+      </c>
+      <c r="C6" s="5" t="inlineStr">
+        <is>
+          <t>required</t>
+        </is>
+      </c>
+      <c r="D6" s="5" t="inlineStr">
+        <is>
+          <t>required</t>
+        </is>
+      </c>
+      <c r="E6" s="5" t="inlineStr">
+        <is>
+          <t>required</t>
+        </is>
+      </c>
+      <c r="F6" s="5" t="inlineStr">
+        <is>
+          <t>required</t>
+        </is>
+      </c>
+      <c r="G6" s="5" t="inlineStr">
+        <is>
+          <t>required</t>
+        </is>
+      </c>
+      <c r="H6" s="5" t="inlineStr">
+        <is>
+          <t>required</t>
+        </is>
+      </c>
+      <c r="I6" s="5" t="inlineStr">
+        <is>
           <t>optional</t>
         </is>
       </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="6" t="n"/>
-      <c r="B6" s="6" t="n"/>
-      <c r="C6" s="6" t="n"/>
-      <c r="D6" s="6" t="n"/>
-      <c r="E6" s="6" t="n"/>
-      <c r="F6" s="6" t="n"/>
-      <c r="G6" s="6" t="n"/>
-      <c r="H6" s="6" t="n"/>
-      <c r="I6" s="6" t="n"/>
     </row>
     <row r="7">
       <c r="A7" s="6" t="n"/>
@@ -19977,6 +20045,17 @@
       <c r="G1005" s="6" t="n"/>
       <c r="H1005" s="6" t="n"/>
       <c r="I1005" s="6" t="n"/>
+    </row>
+    <row r="1006">
+      <c r="A1006" s="6" t="n"/>
+      <c r="B1006" s="6" t="n"/>
+      <c r="C1006" s="6" t="n"/>
+      <c r="D1006" s="6" t="n"/>
+      <c r="E1006" s="6" t="n"/>
+      <c r="F1006" s="6" t="n"/>
+      <c r="G1006" s="6" t="n"/>
+      <c r="H1006" s="6" t="n"/>
+      <c r="I1006" s="6" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -19990,7 +20069,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1005"/>
+  <dimension ref="A1:F1006"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -20137,42 +20216,66 @@
     <row r="5">
       <c r="A5" s="8" t="inlineStr">
         <is>
-          <t>required</t>
+          <t>unrestricted</t>
         </is>
       </c>
       <c r="B5" s="8" t="inlineStr">
         <is>
-          <t>required</t>
+          <t>unrestricted</t>
         </is>
       </c>
       <c r="C5" s="8" t="inlineStr">
         <is>
-          <t>required</t>
+          <t>unrestricted</t>
         </is>
       </c>
       <c r="D5" s="8" t="inlineStr">
         <is>
-          <t>required</t>
+          <t>unrestricted</t>
         </is>
       </c>
       <c r="E5" s="8" t="inlineStr">
         <is>
-          <t>required</t>
+          <t>unrestricted</t>
         </is>
       </c>
       <c r="F5" s="8" t="inlineStr">
         <is>
+          <t>unrestricted</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="8" t="inlineStr">
+        <is>
+          <t>required</t>
+        </is>
+      </c>
+      <c r="B6" s="8" t="inlineStr">
+        <is>
+          <t>required</t>
+        </is>
+      </c>
+      <c r="C6" s="8" t="inlineStr">
+        <is>
+          <t>required</t>
+        </is>
+      </c>
+      <c r="D6" s="8" t="inlineStr">
+        <is>
+          <t>required</t>
+        </is>
+      </c>
+      <c r="E6" s="8" t="inlineStr">
+        <is>
+          <t>required</t>
+        </is>
+      </c>
+      <c r="F6" s="8" t="inlineStr">
+        <is>
           <t>optional</t>
         </is>
       </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="9" t="n"/>
-      <c r="B6" s="9" t="n"/>
-      <c r="C6" s="9" t="n"/>
-      <c r="D6" s="9" t="n"/>
-      <c r="E6" s="9" t="n"/>
-      <c r="F6" s="9" t="n"/>
     </row>
     <row r="7">
       <c r="A7" s="9" t="n"/>
@@ -28165,6 +28268,14 @@
       <c r="D1005" s="9" t="n"/>
       <c r="E1005" s="9" t="n"/>
       <c r="F1005" s="9" t="n"/>
+    </row>
+    <row r="1006">
+      <c r="A1006" s="9" t="n"/>
+      <c r="B1006" s="9" t="n"/>
+      <c r="C1006" s="9" t="n"/>
+      <c r="D1006" s="9" t="n"/>
+      <c r="E1006" s="9" t="n"/>
+      <c r="F1006" s="9" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -28178,7 +28289,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I1005"/>
+  <dimension ref="A1:I1006"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -28388,60 +28499,96 @@
     <row r="5">
       <c r="A5" s="11" t="inlineStr">
         <is>
-          <t>required</t>
+          <t>unrestricted</t>
         </is>
       </c>
       <c r="B5" s="11" t="inlineStr">
         <is>
-          <t>required</t>
+          <t>unrestricted</t>
         </is>
       </c>
       <c r="C5" s="11" t="inlineStr">
         <is>
-          <t>required</t>
+          <t>unrestricted</t>
         </is>
       </c>
       <c r="D5" s="11" t="inlineStr">
         <is>
-          <t>required</t>
+          <t>unrestricted</t>
         </is>
       </c>
       <c r="E5" s="11" t="inlineStr">
         <is>
-          <t>recommended</t>
+          <t>unrestricted</t>
         </is>
       </c>
       <c r="F5" s="11" t="inlineStr">
         <is>
-          <t>required</t>
+          <t>unrestricted</t>
         </is>
       </c>
       <c r="G5" s="11" t="inlineStr">
         <is>
-          <t>required</t>
+          <t>unrestricted</t>
         </is>
       </c>
       <c r="H5" s="11" t="inlineStr">
         <is>
-          <t>recommended</t>
+          <t>unrestricted</t>
         </is>
       </c>
       <c r="I5" s="11" t="inlineStr">
         <is>
+          <t>unrestricted</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="11" t="inlineStr">
+        <is>
+          <t>required</t>
+        </is>
+      </c>
+      <c r="B6" s="11" t="inlineStr">
+        <is>
+          <t>required</t>
+        </is>
+      </c>
+      <c r="C6" s="11" t="inlineStr">
+        <is>
+          <t>required</t>
+        </is>
+      </c>
+      <c r="D6" s="11" t="inlineStr">
+        <is>
+          <t>required</t>
+        </is>
+      </c>
+      <c r="E6" s="11" t="inlineStr">
+        <is>
+          <t>recommended</t>
+        </is>
+      </c>
+      <c r="F6" s="11" t="inlineStr">
+        <is>
+          <t>required</t>
+        </is>
+      </c>
+      <c r="G6" s="11" t="inlineStr">
+        <is>
+          <t>required</t>
+        </is>
+      </c>
+      <c r="H6" s="11" t="inlineStr">
+        <is>
+          <t>recommended</t>
+        </is>
+      </c>
+      <c r="I6" s="11" t="inlineStr">
+        <is>
           <t>optional</t>
         </is>
       </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="12" t="n"/>
-      <c r="B6" s="12" t="n"/>
-      <c r="C6" s="12" t="n"/>
-      <c r="D6" s="12" t="n"/>
-      <c r="E6" s="12" t="n"/>
-      <c r="F6" s="12" t="n"/>
-      <c r="G6" s="12" t="n"/>
-      <c r="H6" s="12" t="n"/>
-      <c r="I6" s="12" t="n"/>
     </row>
     <row r="7">
       <c r="A7" s="12" t="n"/>
@@ -39431,6 +39578,17 @@
       <c r="G1005" s="12" t="n"/>
       <c r="H1005" s="12" t="n"/>
       <c r="I1005" s="12" t="n"/>
+    </row>
+    <row r="1006">
+      <c r="A1006" s="12" t="n"/>
+      <c r="B1006" s="12" t="n"/>
+      <c r="C1006" s="12" t="n"/>
+      <c r="D1006" s="12" t="n"/>
+      <c r="E1006" s="12" t="n"/>
+      <c r="F1006" s="12" t="n"/>
+      <c r="G1006" s="12" t="n"/>
+      <c r="H1006" s="12" t="n"/>
+      <c r="I1006" s="12" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -39444,7 +39602,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D1005"/>
+  <dimension ref="A1:D1006"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -39549,30 +39707,46 @@
     <row r="5">
       <c r="A5" s="14" t="inlineStr">
         <is>
-          <t>required</t>
+          <t>unrestricted</t>
         </is>
       </c>
       <c r="B5" s="14" t="inlineStr">
         <is>
-          <t>required</t>
+          <t>unrestricted</t>
         </is>
       </c>
       <c r="C5" s="14" t="inlineStr">
         <is>
-          <t>optional</t>
+          <t>unrestricted</t>
         </is>
       </c>
       <c r="D5" s="14" t="inlineStr">
         <is>
+          <t>unrestricted</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="14" t="inlineStr">
+        <is>
+          <t>required</t>
+        </is>
+      </c>
+      <c r="B6" s="14" t="inlineStr">
+        <is>
+          <t>required</t>
+        </is>
+      </c>
+      <c r="C6" s="14" t="inlineStr">
+        <is>
           <t>optional</t>
         </is>
       </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="15" t="n"/>
-      <c r="B6" s="15" t="n"/>
-      <c r="C6" s="15" t="n"/>
-      <c r="D6" s="15" t="n"/>
+      <c r="D6" s="14" t="inlineStr">
+        <is>
+          <t>optional</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="15" t="n"/>
@@ -45567,6 +45741,12 @@
       <c r="B1005" s="15" t="n"/>
       <c r="C1005" s="15" t="n"/>
       <c r="D1005" s="15" t="n"/>
+    </row>
+    <row r="1006">
+      <c r="A1006" s="15" t="n"/>
+      <c r="B1006" s="15" t="n"/>
+      <c r="C1006" s="15" t="n"/>
+      <c r="D1006" s="15" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -45580,7 +45760,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H1005"/>
+  <dimension ref="A1:H1006"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -45769,54 +45949,86 @@
     <row r="5">
       <c r="A5" s="2" t="inlineStr">
         <is>
-          <t>optional</t>
+          <t>unrestricted</t>
         </is>
       </c>
       <c r="B5" s="2" t="inlineStr">
         <is>
-          <t>optional</t>
+          <t>unrestricted</t>
         </is>
       </c>
       <c r="C5" s="2" t="inlineStr">
         <is>
-          <t>optional</t>
+          <t>unrestricted</t>
         </is>
       </c>
       <c r="D5" s="2" t="inlineStr">
         <is>
-          <t>optional</t>
+          <t>unrestricted</t>
         </is>
       </c>
       <c r="E5" s="2" t="inlineStr">
         <is>
-          <t>optional</t>
+          <t>unrestricted</t>
         </is>
       </c>
       <c r="F5" s="2" t="inlineStr">
         <is>
-          <t>required</t>
+          <t>unrestricted</t>
         </is>
       </c>
       <c r="G5" s="2" t="inlineStr">
         <is>
-          <t>required</t>
+          <t>unrestricted</t>
         </is>
       </c>
       <c r="H5" s="2" t="inlineStr">
         <is>
+          <t>unrestricted</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="inlineStr">
+        <is>
           <t>optional</t>
         </is>
       </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="3" t="n"/>
-      <c r="B6" s="3" t="n"/>
-      <c r="C6" s="3" t="n"/>
-      <c r="D6" s="3" t="n"/>
-      <c r="E6" s="3" t="n"/>
-      <c r="F6" s="3" t="n"/>
-      <c r="G6" s="3" t="n"/>
-      <c r="H6" s="3" t="n"/>
+      <c r="B6" s="2" t="inlineStr">
+        <is>
+          <t>optional</t>
+        </is>
+      </c>
+      <c r="C6" s="2" t="inlineStr">
+        <is>
+          <t>optional</t>
+        </is>
+      </c>
+      <c r="D6" s="2" t="inlineStr">
+        <is>
+          <t>optional</t>
+        </is>
+      </c>
+      <c r="E6" s="2" t="inlineStr">
+        <is>
+          <t>optional</t>
+        </is>
+      </c>
+      <c r="F6" s="2" t="inlineStr">
+        <is>
+          <t>required</t>
+        </is>
+      </c>
+      <c r="G6" s="2" t="inlineStr">
+        <is>
+          <t>required</t>
+        </is>
+      </c>
+      <c r="H6" s="2" t="inlineStr">
+        <is>
+          <t>optional</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="3" t="n"/>
@@ -55807,6 +56019,16 @@
       <c r="F1005" s="3" t="n"/>
       <c r="G1005" s="3" t="n"/>
       <c r="H1005" s="3" t="n"/>
+    </row>
+    <row r="1006">
+      <c r="A1006" s="3" t="n"/>
+      <c r="B1006" s="3" t="n"/>
+      <c r="C1006" s="3" t="n"/>
+      <c r="D1006" s="3" t="n"/>
+      <c r="E1006" s="3" t="n"/>
+      <c r="F1006" s="3" t="n"/>
+      <c r="G1006" s="3" t="n"/>
+      <c r="H1006" s="3" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Fix value restriction generation
</commit_message>
<xml_diff>
--- a/spreadsheets/ghga_submission_minimal.xlsx
+++ b/spreadsheets/ghga_submission_minimal.xlsx
@@ -698,7 +698,7 @@
       </c>
       <c r="D5" s="2" t="inlineStr">
         <is>
-          <t>unrestricted</t>
+          <t>controlled vocabulary</t>
         </is>
       </c>
       <c r="E5" s="2" t="inlineStr">
@@ -8892,7 +8892,7 @@
       </c>
       <c r="E3" s="5" t="inlineStr">
         <is>
-          <t>type: string</t>
+          <t>type: integer</t>
         </is>
       </c>
       <c r="F3" s="5" t="inlineStr">
@@ -8971,7 +8971,7 @@
       </c>
       <c r="B5" s="5" t="inlineStr">
         <is>
-          <t>unrestricted</t>
+          <t>restriction: value from Study.alias</t>
         </is>
       </c>
       <c r="C5" s="5" t="inlineStr">
@@ -8981,7 +8981,7 @@
       </c>
       <c r="D5" s="5" t="inlineStr">
         <is>
-          <t>unrestricted</t>
+          <t>controlled vocabulary</t>
         </is>
       </c>
       <c r="E5" s="5" t="inlineStr">
@@ -9001,7 +9001,7 @@
       </c>
       <c r="H5" s="5" t="inlineStr">
         <is>
-          <t>unrestricted</t>
+          <t>restriction: value from Dataset.alias</t>
         </is>
       </c>
       <c r="I5" s="5" t="inlineStr">
@@ -20236,7 +20236,7 @@
       </c>
       <c r="E5" s="8" t="inlineStr">
         <is>
-          <t>unrestricted</t>
+          <t>restriction: value from DataAccessPolicy.alias</t>
         </is>
       </c>
       <c r="F5" s="8" t="inlineStr">
@@ -28524,17 +28524,17 @@
       </c>
       <c r="F5" s="11" t="inlineStr">
         <is>
-          <t>unrestricted</t>
+          <t>restriction: value from DataAccessCommittee.alias</t>
         </is>
       </c>
       <c r="G5" s="11" t="inlineStr">
         <is>
-          <t>unrestricted</t>
+          <t>controlled vocabulary</t>
         </is>
       </c>
       <c r="H5" s="11" t="inlineStr">
         <is>
-          <t>unrestricted</t>
+          <t>controlled vocabulary</t>
         </is>
       </c>
       <c r="I5" s="11" t="inlineStr">
@@ -45880,7 +45880,7 @@
       </c>
       <c r="D3" s="2" t="inlineStr">
         <is>
-          <t>type: string</t>
+          <t>type: integer</t>
         </is>
       </c>
       <c r="E3" s="2" t="inlineStr">
@@ -45979,7 +45979,7 @@
       </c>
       <c r="G5" s="2" t="inlineStr">
         <is>
-          <t>unrestricted</t>
+          <t>restriction: value from Study.alias</t>
         </is>
       </c>
       <c r="H5" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Fix value restriction generation (#124)
</commit_message>
<xml_diff>
--- a/spreadsheets/ghga_submission_minimal.xlsx
+++ b/spreadsheets/ghga_submission_minimal.xlsx
@@ -698,7 +698,7 @@
       </c>
       <c r="D5" s="2" t="inlineStr">
         <is>
-          <t>unrestricted</t>
+          <t>controlled vocabulary</t>
         </is>
       </c>
       <c r="E5" s="2" t="inlineStr">
@@ -8892,7 +8892,7 @@
       </c>
       <c r="E3" s="5" t="inlineStr">
         <is>
-          <t>type: string</t>
+          <t>type: integer</t>
         </is>
       </c>
       <c r="F3" s="5" t="inlineStr">
@@ -8971,7 +8971,7 @@
       </c>
       <c r="B5" s="5" t="inlineStr">
         <is>
-          <t>unrestricted</t>
+          <t>restriction: value from Study.alias</t>
         </is>
       </c>
       <c r="C5" s="5" t="inlineStr">
@@ -8981,7 +8981,7 @@
       </c>
       <c r="D5" s="5" t="inlineStr">
         <is>
-          <t>unrestricted</t>
+          <t>controlled vocabulary</t>
         </is>
       </c>
       <c r="E5" s="5" t="inlineStr">
@@ -9001,7 +9001,7 @@
       </c>
       <c r="H5" s="5" t="inlineStr">
         <is>
-          <t>unrestricted</t>
+          <t>restriction: value from Dataset.alias</t>
         </is>
       </c>
       <c r="I5" s="5" t="inlineStr">
@@ -20236,7 +20236,7 @@
       </c>
       <c r="E5" s="8" t="inlineStr">
         <is>
-          <t>unrestricted</t>
+          <t>restriction: value from DataAccessPolicy.alias</t>
         </is>
       </c>
       <c r="F5" s="8" t="inlineStr">
@@ -28524,17 +28524,17 @@
       </c>
       <c r="F5" s="11" t="inlineStr">
         <is>
-          <t>unrestricted</t>
+          <t>restriction: value from DataAccessCommittee.alias</t>
         </is>
       </c>
       <c r="G5" s="11" t="inlineStr">
         <is>
-          <t>unrestricted</t>
+          <t>controlled vocabulary</t>
         </is>
       </c>
       <c r="H5" s="11" t="inlineStr">
         <is>
-          <t>unrestricted</t>
+          <t>controlled vocabulary</t>
         </is>
       </c>
       <c r="I5" s="11" t="inlineStr">
@@ -45880,7 +45880,7 @@
       </c>
       <c r="D3" s="2" t="inlineStr">
         <is>
-          <t>type: string</t>
+          <t>type: integer</t>
         </is>
       </c>
       <c r="E3" s="2" t="inlineStr">
@@ -45979,7 +45979,7 @@
       </c>
       <c r="G5" s="2" t="inlineStr">
         <is>
-          <t>unrestricted</t>
+          <t>restriction: value from Study.alias</t>
         </is>
       </c>
       <c r="H5" s="2" t="inlineStr">

</xml_diff>

<commit_message>
several minor fixes (slot order, requirement, CVs)
</commit_message>
<xml_diff>
--- a/spreadsheets/ghga_submission_minimal.xlsx
+++ b/spreadsheets/ghga_submission_minimal.xlsx
@@ -8808,12 +8808,12 @@
       </c>
       <c r="G1" s="4" t="inlineStr">
         <is>
-          <t>forward_or_reverse</t>
+          <t>checksum_type</t>
         </is>
       </c>
       <c r="H1" s="4" t="inlineStr">
         <is>
-          <t>checksum_type</t>
+          <t>forward_or_reverse</t>
         </is>
       </c>
       <c r="I1" s="4" t="inlineStr">
@@ -8855,12 +8855,12 @@
       </c>
       <c r="G2" s="5" t="inlineStr">
         <is>
-          <t>Denotes whether a submitted FASTQ file contains forward (R1) or reverse (R2) reads for paired-end sequencing. The number that identifies each read direction in a paired-end nucleotide sequencing reaction.</t>
+          <t>The type of algorithm used to generate the checksum of a file.</t>
         </is>
       </c>
       <c r="H2" s="5" t="inlineStr">
         <is>
-          <t>The type of algorithm used to generate the checksum of a file.</t>
+          <t>Denotes whether a submitted FASTQ file contains forward (R1) or reverse (R2) reads for paired-end sequencing. The number that identifies each read direction in a paired-end nucleotide sequencing reaction.</t>
         </is>
       </c>
       <c r="I2" s="5" t="inlineStr">
@@ -8996,12 +8996,12 @@
       </c>
       <c r="G5" s="5" t="inlineStr">
         <is>
-          <t>controlled vocabulary</t>
+          <t>unrestricted</t>
         </is>
       </c>
       <c r="H5" s="5" t="inlineStr">
         <is>
-          <t>unrestricted</t>
+          <t>controlled vocabulary</t>
         </is>
       </c>
       <c r="I5" s="5" t="inlineStr">
@@ -9043,12 +9043,12 @@
       </c>
       <c r="G6" s="5" t="inlineStr">
         <is>
-          <t>recommended</t>
+          <t>required</t>
         </is>
       </c>
       <c r="H6" s="5" t="inlineStr">
         <is>
-          <t>required</t>
+          <t>recommended</t>
         </is>
       </c>
       <c r="I6" s="5" t="inlineStr">
@@ -27304,17 +27304,17 @@
       </c>
       <c r="F1" s="10" t="inlineStr">
         <is>
-          <t>data_access_committee</t>
+          <t>data_use_permission</t>
         </is>
       </c>
       <c r="G1" s="10" t="inlineStr">
         <is>
-          <t>data_use_permission</t>
+          <t>data_use_modifiers</t>
         </is>
       </c>
       <c r="H1" s="10" t="inlineStr">
         <is>
-          <t>data_use_modifiers</t>
+          <t>data_access_committee</t>
         </is>
       </c>
     </row>
@@ -27346,17 +27346,17 @@
       </c>
       <c r="F2" s="11" t="inlineStr">
         <is>
-          <t>The Data Access Committee linked to this policy.</t>
+          <t>Data use permission associated with a policy. Typically one or more terms from DUO and should be descendants of 'DUO:0000001 data use permission'. Please use 'DUO:0000026' if no other permission applies.</t>
         </is>
       </c>
       <c r="G2" s="11" t="inlineStr">
         <is>
-          <t>Data use permission associated with a policy. Typically one or more terms from DUO and should be descendants of 'DUO:0000001 data use permission'.</t>
+          <t>Modifier for Data use permission associated with a policy. Should be descendants of 'DUO:0000017 data use modifier'</t>
         </is>
       </c>
       <c r="H2" s="11" t="inlineStr">
         <is>
-          <t>Modifier for Data use permission associated with a policy. Should be descendants of 'DUO:0000017 data use modifier'</t>
+          <t>The Data Access Committee linked to this policy.</t>
         </is>
       </c>
     </row>
@@ -27435,12 +27435,12 @@
       </c>
       <c r="G4" s="11" t="inlineStr">
         <is>
-          <t>single value</t>
+          <t>multiple values</t>
         </is>
       </c>
       <c r="H4" s="11" t="inlineStr">
         <is>
-          <t>multiple values</t>
+          <t>single value</t>
         </is>
       </c>
     </row>
@@ -27472,7 +27472,7 @@
       </c>
       <c r="F5" s="11" t="inlineStr">
         <is>
-          <t>restriction: value from DataAccessCommittee.alias</t>
+          <t>controlled vocabulary</t>
         </is>
       </c>
       <c r="G5" s="11" t="inlineStr">
@@ -27482,7 +27482,7 @@
       </c>
       <c r="H5" s="11" t="inlineStr">
         <is>
-          <t>controlled vocabulary</t>
+          <t>restriction: value from DataAccessCommittee.alias</t>
         </is>
       </c>
     </row>
@@ -27519,12 +27519,12 @@
       </c>
       <c r="G6" s="11" t="inlineStr">
         <is>
-          <t>required</t>
+          <t>recommended</t>
         </is>
       </c>
       <c r="H6" s="11" t="inlineStr">
         <is>
-          <t>recommended</t>
+          <t>required</t>
         </is>
       </c>
     </row>
@@ -42724,12 +42724,12 @@
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>study</t>
+          <t>xref</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>xref</t>
+          <t>study</t>
         </is>
       </c>
     </row>
@@ -42771,12 +42771,12 @@
       </c>
       <c r="H2" s="2" t="inlineStr">
         <is>
-          <t>The Study entity associated with this Publication.</t>
+          <t>One or more cross-references for this Publication.</t>
         </is>
       </c>
       <c r="I2" s="2" t="inlineStr">
         <is>
-          <t>One or more cross-references for this Publication.</t>
+          <t>The Study entity associated with this Publication.</t>
         </is>
       </c>
     </row>
@@ -42865,12 +42865,12 @@
       </c>
       <c r="H4" s="2" t="inlineStr">
         <is>
-          <t>single value</t>
+          <t>multiple values</t>
         </is>
       </c>
       <c r="I4" s="2" t="inlineStr">
         <is>
-          <t>multiple values</t>
+          <t>single value</t>
         </is>
       </c>
     </row>
@@ -42912,12 +42912,12 @@
       </c>
       <c r="H5" s="2" t="inlineStr">
         <is>
-          <t>restriction: value from Study.alias</t>
+          <t>unrestricted</t>
         </is>
       </c>
       <c r="I5" s="2" t="inlineStr">
         <is>
-          <t>unrestricted</t>
+          <t>restriction: value from Study.alias</t>
         </is>
       </c>
     </row>
@@ -42959,12 +42959,12 @@
       </c>
       <c r="H6" s="2" t="inlineStr">
         <is>
-          <t>required</t>
+          <t>optional</t>
         </is>
       </c>
       <c r="I6" s="2" t="inlineStr">
         <is>
-          <t>optional</t>
+          <t>required</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
updated descriptions and generated artifacts
</commit_message>
<xml_diff>
--- a/spreadsheets/ghga_submission_minimal.xlsx
+++ b/spreadsheets/ghga_submission_minimal.xlsx
@@ -592,7 +592,7 @@
       </c>
       <c r="B2" s="2" t="inlineStr">
         <is>
-          <t>A comprehensive title for the study.</t>
+          <t>A comprehensive title for the Study.</t>
         </is>
       </c>
       <c r="C2" s="2" t="inlineStr">
@@ -602,7 +602,7 @@
       </c>
       <c r="D2" s="2" t="inlineStr">
         <is>
-          <t>The type of Study. For example, 'Cancer Genomics', 'Epigenetics', 'Exome Sequencing'.</t>
+          <t>The type of Study, e.g. 'Cancer Genomics', 'Epigenetics', 'Exome Sequencing'.</t>
         </is>
       </c>
       <c r="E2" s="2" t="inlineStr">
@@ -612,7 +612,7 @@
       </c>
       <c r="F2" s="2" t="inlineStr">
         <is>
-          <t>Custom key/value pairs that further characterizes the Study. (e.g.: approaches - single-cell,_bulk_etc)</t>
+          <t>One or more attributes that further characterize this Study.</t>
         </is>
       </c>
     </row>
@@ -8840,7 +8840,7 @@
       </c>
       <c r="D2" s="5" t="inlineStr">
         <is>
-          <t>The format of the file: BAM, SAM, CRAM, BAI, etc.</t>
+          <t>The format of the file, e.g. BAM, SAM, CRAM, BAI.</t>
         </is>
       </c>
       <c r="E2" s="5" t="inlineStr">
@@ -20119,7 +20119,7 @@
       </c>
       <c r="B2" s="8" t="inlineStr">
         <is>
-          <t>A title for the submitted Dataset.</t>
+          <t>A title for the Dataset.</t>
         </is>
       </c>
       <c r="C2" s="8" t="inlineStr">
@@ -20129,7 +20129,7 @@
       </c>
       <c r="D2" s="8" t="inlineStr">
         <is>
-          <t>The type of a dataset.</t>
+          <t>The type of the Dataset.</t>
         </is>
       </c>
       <c r="E2" s="8" t="inlineStr">
@@ -27336,22 +27336,22 @@
       </c>
       <c r="D2" s="11" t="inlineStr">
         <is>
-          <t>The terms of data use and policy verbiage should be captured here.</t>
+          <t>The complete text for the Data Access Policy.</t>
         </is>
       </c>
       <c r="E2" s="11" t="inlineStr">
         <is>
-          <t>URL for the policy, if available. This is useful if the terms of the policy is made available online at a resolvable URL.</t>
+          <t>An alternative to pasting the Data Access Policy text is to provide the URL for the policy, if available. This is useful if the terms of the policy is made available online at a resolvable URL.</t>
         </is>
       </c>
       <c r="F2" s="11" t="inlineStr">
         <is>
-          <t>Data use permission associated with a policy. Typically one or more terms from DUO and should be descendants of 'DUO:0000001 data use permission'. Please use 'DUO:0000026' if no other permission applies.</t>
+          <t>Data use permission associated with an entity. Typically one or more terms from DUO. Should be descendants of 'DUO:0000001 data use permission'.  Please use 'DUO:0000026' if no other permission applies.</t>
         </is>
       </c>
       <c r="G2" s="11" t="inlineStr">
         <is>
-          <t>Modifier for Data use permission associated with a policy. Should be descendants of 'DUO:0000017 data use modifier'</t>
+          <t>Modifier for Data use permission associated with an entity. Should be descendants of 'DUO:0000017 data use modifier'</t>
         </is>
       </c>
       <c r="H2" s="11" t="inlineStr">
@@ -42766,7 +42766,7 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>DOI identifier of the Publication.</t>
+          <t>DOI identifier of a publication.</t>
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">

</xml_diff>

<commit_message>
updated request for changes; updated artifacts
</commit_message>
<xml_diff>
--- a/spreadsheets/ghga_submission_minimal.xlsx
+++ b/spreadsheets/ghga_submission_minimal.xlsx
@@ -592,7 +592,7 @@
       </c>
       <c r="B2" s="2" t="inlineStr">
         <is>
-          <t>A comprehensive title for the Study.</t>
+          <t>A comprehensive title for this Study.</t>
         </is>
       </c>
       <c r="C2" s="2" t="inlineStr">
@@ -602,7 +602,7 @@
       </c>
       <c r="D2" s="2" t="inlineStr">
         <is>
-          <t>The type of Study, e.g. 'Cancer Genomics', 'Epigenetics', 'Exome Sequencing'.</t>
+          <t>The type of this Study (e.g., Cancer Genomics, Epigenetics, Exome Sequencing).</t>
         </is>
       </c>
       <c r="E2" s="2" t="inlineStr">
@@ -8830,7 +8830,7 @@
       </c>
       <c r="B2" s="5" t="inlineStr">
         <is>
-          <t>The Study that is associated with this StudyFile.</t>
+          <t>The Study that is associated with this Study File.</t>
         </is>
       </c>
       <c r="C2" s="5" t="inlineStr">
@@ -8840,22 +8840,22 @@
       </c>
       <c r="D2" s="5" t="inlineStr">
         <is>
-          <t>The format of the file, e.g. BAM, SAM, CRAM, BAI.</t>
+          <t>The format of the File (e.g., BAM, SAM, CRAM, BAI).</t>
         </is>
       </c>
       <c r="E2" s="5" t="inlineStr">
         <is>
-          <t>The size of a file in bytes.</t>
+          <t>The size of the File in bytes.</t>
         </is>
       </c>
       <c r="F2" s="5" t="inlineStr">
         <is>
-          <t>A computed value which depends on the contents of a block of data and which is transmitted or stored along with the data in order to detect corruption of the data. The receiving system recomputes the checksum based upon the received data and compares this value with the one sent with the data. If the two values are the same, the receiver has some confidence that the data was received correctly.</t>
+          <t>The checksum of the File.</t>
         </is>
       </c>
       <c r="G2" s="5" t="inlineStr">
         <is>
-          <t>The type of algorithm used to generate the checksum of a file.</t>
+          <t>The type of algorithm used to generate the checksum of the File.</t>
         </is>
       </c>
       <c r="H2" s="5" t="inlineStr">
@@ -20119,7 +20119,7 @@
       </c>
       <c r="B2" s="8" t="inlineStr">
         <is>
-          <t>A title for the Dataset.</t>
+          <t>A title for this Dataset.</t>
         </is>
       </c>
       <c r="C2" s="8" t="inlineStr">
@@ -20129,7 +20129,7 @@
       </c>
       <c r="D2" s="8" t="inlineStr">
         <is>
-          <t>The type of the Dataset.</t>
+          <t>The type of this Dataset.</t>
         </is>
       </c>
       <c r="E2" s="8" t="inlineStr">
@@ -27326,12 +27326,12 @@
       </c>
       <c r="B2" s="11" t="inlineStr">
         <is>
-          <t>A name for the Data Access Policy.</t>
+          <t>A name for this Data Access Policy.</t>
         </is>
       </c>
       <c r="C2" s="11" t="inlineStr">
         <is>
-          <t>A short description for the Data Access Policy.</t>
+          <t>A short description for this Data Access Policy.</t>
         </is>
       </c>
       <c r="D2" s="11" t="inlineStr">
@@ -27341,22 +27341,22 @@
       </c>
       <c r="E2" s="11" t="inlineStr">
         <is>
-          <t>An alternative to pasting the Data Access Policy text is to provide the URL for the policy, if available. This is useful if the terms of the policy is made available online at a resolvable URL.</t>
+          <t>An alternative to the Data Access Policy text is to provide the URL for the policy. This is useful if the terms of the policy are available online at a resolvable URL.</t>
         </is>
       </c>
       <c r="F2" s="11" t="inlineStr">
         <is>
-          <t>Data use permission associated with a Data Use Policy. Typically one or more terms from DUO and should be descendants of 'DUO:0000001 data use permission'. Please use 'DUO:0000006' if no other permission applies.</t>
+          <t>The Data Use Permission associated with this Data Use Policy. The used term should be a descendant of 'DUO:0000001: data use permission'.</t>
         </is>
       </c>
       <c r="G2" s="11" t="inlineStr">
         <is>
-          <t>Modifier for the Data Use Permission associated with a Data Use Policy. Should be descendants of 'DUO:0000017 data use modifier'. Please use 'DUO:0000026' if no other modifier applies.</t>
+          <t>One or more Data Use Modifiers for the Data Use Permission associated with this Data Use Policy. The used terms should be descendants of 'DUO:0000017: data use modifier'. Please use 'user specific restriction' if no other modifier applies.</t>
         </is>
       </c>
       <c r="H2" s="11" t="inlineStr">
         <is>
-          <t>The Data Access Committee linked to this policy.</t>
+          <t>The Data Access Committee linked to this Data Use Policy.</t>
         </is>
       </c>
     </row>
@@ -37578,12 +37578,12 @@
       </c>
       <c r="B2" s="14" t="inlineStr">
         <is>
-          <t>The email of the Data Access Committee. Please do not enter personal email addresses!</t>
+          <t>The email of the Data Access Committee (e.g., DAC[at]email.com). This property must not include any personally identifiable data.</t>
         </is>
       </c>
       <c r="C2" s="14" t="inlineStr">
         <is>
-          <t>The institute a person is affiliated with.</t>
+          <t>The Institute a person is affiliated with.</t>
         </is>
       </c>
     </row>
@@ -42741,27 +42741,27 @@
       </c>
       <c r="B2" s="2" t="inlineStr">
         <is>
-          <t>The title for the Publication.</t>
+          <t>The title for this Publication.</t>
         </is>
       </c>
       <c r="C2" s="2" t="inlineStr">
         <is>
-          <t>The study abstract that describes the goals. Can also hold abstract from a publication related to this study.</t>
+          <t>The study abstract that describes the goals. Can also hold abstract from a Publication related to this Study.</t>
         </is>
       </c>
       <c r="D2" s="2" t="inlineStr">
         <is>
-          <t>Author(s) of the associated Publication.</t>
+          <t>Author(s) of this Publication.</t>
         </is>
       </c>
       <c r="E2" s="2" t="inlineStr">
         <is>
-          <t>Year in which the paper was published.</t>
+          <t>The year in which the paper was published.</t>
         </is>
       </c>
       <c r="F2" s="2" t="inlineStr">
         <is>
-          <t>Name of the journal.</t>
+          <t>The name of the journal.</t>
         </is>
       </c>
       <c r="G2" s="2" t="inlineStr">

</xml_diff>

<commit_message>
implemented requested changes; updated artifacts
</commit_message>
<xml_diff>
--- a/spreadsheets/ghga_submission_minimal.xlsx
+++ b/spreadsheets/ghga_submission_minimal.xlsx
@@ -570,7 +570,7 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>type</t>
+          <t>types</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
@@ -602,7 +602,7 @@
       </c>
       <c r="D2" s="2" t="inlineStr">
         <is>
-          <t>The type of this Study (e.g., Cancer Genomics, Epigenetics, Exome Sequencing).</t>
+          <t>One or more types of this Study (e.g., Cancer Genomics, Epigenetics, Exome Sequencing).</t>
         </is>
       </c>
       <c r="E2" s="2" t="inlineStr">

</xml_diff>